<commit_message>
Adding streamed sobel grad and mag calculation
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>apply_gaussian_kernel</t>
   </si>
@@ -65,14 +65,20 @@
     <t>daimler_800_410</t>
   </si>
   <si>
-    <t>GPU (sobels)</t>
+    <t>GPU (stream for mag/dir)</t>
+  </si>
+  <si>
+    <t>GPU (stream for sobel x / y)</t>
+  </si>
+  <si>
+    <t>changes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -80,16 +86,41 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -97,17 +128,40 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Calculation" xfId="2" builtinId="22"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -386,25 +440,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" customWidth="1"/>
+    <col min="4" max="5" width="25.7109375" customWidth="1"/>
+    <col min="6" max="6" width="24.7109375" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>9</v>
       </c>
@@ -412,10 +468,19 @@
         <v>10</v>
       </c>
       <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -428,8 +493,11 @@
       <c r="D3">
         <v>0.19827</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F3">
+        <v>0.19964999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -442,8 +510,11 @@
       <c r="D4">
         <v>0.19250999999999999</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F4">
+        <v>0.19980999999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -456,8 +527,19 @@
       <c r="D5">
         <v>1.0200000000000001E-3</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" s="2">
+        <f>SUM(C5:C7) - SUM(D5:D7)</f>
+        <v>0.68220999999999998</v>
+      </c>
+      <c r="F5">
+        <v>8.3000000000000001E-4</v>
+      </c>
+      <c r="G5" s="2">
+        <f>SUM(D5:D9) - SUM(F5:F9)</f>
+        <v>0.24640000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -470,8 +552,13 @@
       <c r="D6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" s="2"/>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -484,8 +571,13 @@
       <c r="D7">
         <v>0.10362</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" s="2"/>
+      <c r="F7">
+        <v>1.09E-3</v>
+      </c>
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -498,8 +590,12 @@
       <c r="D8">
         <v>0.16186</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -512,8 +608,12 @@
       <c r="D9">
         <v>6.6619999999999999E-2</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F9">
+        <v>8.48E-2</v>
+      </c>
+      <c r="G9" s="2"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -526,8 +626,11 @@
       <c r="D10">
         <v>9.2700000000000005E-2</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F10">
+        <v>9.2060000000000003E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -540,37 +643,54 @@
       <c r="D11">
         <v>0.16342000000000001</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="F11">
+        <v>0.11866</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="3">
         <f>SUM(B3:B11)</f>
         <v>106.54000000000002</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="3">
         <f>SUM(C3:C11)</f>
         <v>1.5194000000000001</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="3">
         <f>SUM(D3:D11)</f>
         <v>0.98002000000000011</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C13">
+      <c r="E12" s="3"/>
+      <c r="F12" s="3">
+        <f>SUM(F3:F11)</f>
+        <v>0.69689999999999996</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3">
         <f>B12/C12</f>
         <v>70.119784125312634</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="3">
         <f>B12/D12</f>
         <v>108.71206710067142</v>
       </c>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3">
+        <f>B12/F12</f>
+        <v>152.87702683311812</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="3">
     <mergeCell ref="B1:C1"/>
+    <mergeCell ref="E5:E7"/>
+    <mergeCell ref="G5:G9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Adding more comments and code cleanup
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>apply_gaussian_kernel</t>
   </si>
@@ -72,13 +72,16 @@
   </si>
   <si>
     <t>changes</t>
+  </si>
+  <si>
+    <t>Speed V/S CPU</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -97,6 +100,14 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -120,7 +131,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -143,26 +154,40 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="3"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="3" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Calculation" xfId="2" builtinId="22"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Total" xfId="3" builtinId="25"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -443,7 +468,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -454,33 +479,39 @@
     <col min="7" max="7" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3"/>
+      <c r="B1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="1"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+      <c r="C1" s="4"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+    </row>
+    <row r="2" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -527,14 +558,14 @@
       <c r="D5">
         <v>1.0200000000000001E-3</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="1">
         <f>SUM(C5:C7) - SUM(D5:D7)</f>
         <v>0.68220999999999998</v>
       </c>
       <c r="F5">
         <v>8.3000000000000001E-4</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5" s="1">
         <f>SUM(D5:D9) - SUM(F5:F9)</f>
         <v>0.24640000000000001</v>
       </c>
@@ -552,11 +583,11 @@
       <c r="D6">
         <v>0</v>
       </c>
-      <c r="E6" s="2"/>
+      <c r="E6" s="1"/>
       <c r="F6">
         <v>0</v>
       </c>
-      <c r="G6" s="2"/>
+      <c r="G6" s="1"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -571,11 +602,11 @@
       <c r="D7">
         <v>0.10362</v>
       </c>
-      <c r="E7" s="2"/>
+      <c r="E7" s="1"/>
       <c r="F7">
         <v>1.09E-3</v>
       </c>
-      <c r="G7" s="2"/>
+      <c r="G7" s="1"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -593,7 +624,7 @@
       <c r="F8">
         <v>0</v>
       </c>
-      <c r="G8" s="2"/>
+      <c r="G8" s="1"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -611,7 +642,7 @@
       <c r="F9">
         <v>8.48E-2</v>
       </c>
-      <c r="G9" s="2"/>
+      <c r="G9" s="1"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -648,40 +679,45 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="2">
         <f>SUM(B3:B11)</f>
         <v>106.54000000000002</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="2">
         <f>SUM(C3:C11)</f>
         <v>1.5194000000000001</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12" s="2">
         <f>SUM(D3:D11)</f>
         <v>0.98002000000000011</v>
       </c>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3">
+      <c r="E12" s="2"/>
+      <c r="F12" s="2">
         <f>SUM(F3:F11)</f>
         <v>0.69689999999999996</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3">
+      <c r="A13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="2">
+        <f>B12/B12</f>
+        <v>1</v>
+      </c>
+      <c r="C13" s="2">
         <f>B12/C12</f>
         <v>70.119784125312634</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D13" s="2">
         <f>B12/D12</f>
         <v>108.71206710067142</v>
       </c>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3">
+      <c r="E13" s="2"/>
+      <c r="F13" s="2">
         <f>B12/F12</f>
         <v>152.87702683311812</v>
       </c>

</xml_diff>

<commit_message>
updating host to compute threshold after gaussian itself
also adding image writing define to main
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="21">
   <si>
     <t>apply_gaussian_kernel</t>
   </si>
@@ -75,6 +75,18 @@
   </si>
   <si>
     <t>Speed V/S CPU</t>
+  </si>
+  <si>
+    <t>Horses_Run_Animals_horse_9192x6012</t>
+  </si>
+  <si>
+    <t>Red_Mazda_2528_1368</t>
+  </si>
+  <si>
+    <t>range_rover_1920_1080</t>
+  </si>
+  <si>
+    <t>daimler_800_777</t>
   </si>
 </sst>
 </file>
@@ -465,18 +477,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:K34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32" customWidth="1"/>
-    <col min="4" max="5" width="25.7109375" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" customWidth="1"/>
     <col min="6" max="6" width="24.7109375" customWidth="1"/>
     <col min="7" max="7" width="12.5703125" customWidth="1"/>
+    <col min="8" max="8" width="15" customWidth="1"/>
+    <col min="9" max="9" width="12.85546875" customWidth="1"/>
+    <col min="10" max="10" width="10.5703125" customWidth="1"/>
+    <col min="11" max="11" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -722,11 +739,404 @@
         <v>152.87702683311812</v>
       </c>
     </row>
+    <row r="22" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="3"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I22" s="4"/>
+      <c r="J22" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="K22" s="4"/>
+    </row>
+    <row r="23" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="3"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I23" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J23" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K23" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>1629.69</v>
+      </c>
+      <c r="E24">
+        <v>17.352029999999999</v>
+      </c>
+      <c r="F24">
+        <v>103.37</v>
+      </c>
+      <c r="G24">
+        <v>1.07213</v>
+      </c>
+      <c r="H24">
+        <v>62.06</v>
+      </c>
+      <c r="I24">
+        <v>0.64866999999999997</v>
+      </c>
+      <c r="J24">
+        <v>18.739999999999998</v>
+      </c>
+      <c r="K24">
+        <v>0.20058000000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25">
+        <v>63.61</v>
+      </c>
+      <c r="E25">
+        <v>12.748799999999999</v>
+      </c>
+      <c r="F25">
+        <v>3.98</v>
+      </c>
+      <c r="G25">
+        <v>0.87002000000000002</v>
+      </c>
+      <c r="H25">
+        <v>2.39</v>
+      </c>
+      <c r="I25">
+        <v>0.51500999999999997</v>
+      </c>
+      <c r="J25">
+        <v>0.72</v>
+      </c>
+      <c r="K25">
+        <v>0.21187</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>1</v>
+      </c>
+      <c r="D26">
+        <v>3192.68</v>
+      </c>
+      <c r="E26">
+        <v>1.6299999999999999E-3</v>
+      </c>
+      <c r="F26">
+        <v>197.6</v>
+      </c>
+      <c r="G26">
+        <v>1.6999999999999999E-3</v>
+      </c>
+      <c r="H26">
+        <v>122.05</v>
+      </c>
+      <c r="I26">
+        <v>1.6999999999999999E-3</v>
+      </c>
+      <c r="J26">
+        <v>35.380000000000003</v>
+      </c>
+      <c r="K26">
+        <v>8.0000000000000004E-4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>2</v>
+      </c>
+      <c r="D27">
+        <v>3135.95</v>
+      </c>
+      <c r="E27">
+        <v>6.7580000000000001E-2</v>
+      </c>
+      <c r="F27">
+        <v>194.29</v>
+      </c>
+      <c r="G27">
+        <v>4.3040000000000002E-2</v>
+      </c>
+      <c r="H27">
+        <v>127.96</v>
+      </c>
+      <c r="I27">
+        <v>0</v>
+      </c>
+      <c r="J27">
+        <v>34.74</v>
+      </c>
+      <c r="K27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>3</v>
+      </c>
+      <c r="D28">
+        <v>254.7</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <v>16.149999999999999</v>
+      </c>
+      <c r="G28">
+        <v>0</v>
+      </c>
+      <c r="H28">
+        <v>11.81</v>
+      </c>
+      <c r="I28">
+        <v>3.0589999999999999E-2</v>
+      </c>
+      <c r="J28">
+        <v>3.01</v>
+      </c>
+      <c r="K28">
+        <v>3.542E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>4</v>
+      </c>
+      <c r="D29">
+        <v>561.04</v>
+      </c>
+      <c r="E29">
+        <v>5.3512599999999999</v>
+      </c>
+      <c r="F29">
+        <v>33.979999999999997</v>
+      </c>
+      <c r="G29">
+        <v>0.33821000000000001</v>
+      </c>
+      <c r="H29">
+        <v>20.36</v>
+      </c>
+      <c r="I29">
+        <v>0</v>
+      </c>
+      <c r="J29">
+        <v>6.32</v>
+      </c>
+      <c r="K29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>5</v>
+      </c>
+      <c r="D30">
+        <v>420.45</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30">
+        <v>21.3</v>
+      </c>
+      <c r="G30">
+        <v>0</v>
+      </c>
+      <c r="H30">
+        <v>15.89</v>
+      </c>
+      <c r="I30">
+        <v>0.2089</v>
+      </c>
+      <c r="J30">
+        <v>4.29</v>
+      </c>
+      <c r="K30">
+        <v>6.2530000000000002E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>7</v>
+      </c>
+      <c r="D31">
+        <v>195.8</v>
+      </c>
+      <c r="E31">
+        <v>2.8958699999999999</v>
+      </c>
+      <c r="F31">
+        <v>10.35</v>
+      </c>
+      <c r="G31">
+        <v>0.18890000000000001</v>
+      </c>
+      <c r="H31">
+        <v>6</v>
+      </c>
+      <c r="I31">
+        <v>0.11165</v>
+      </c>
+      <c r="J31">
+        <v>1.92</v>
+      </c>
+      <c r="K31">
+        <v>3.5650000000000001E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>8</v>
+      </c>
+      <c r="D32">
+        <v>209.98</v>
+      </c>
+      <c r="E32">
+        <v>8.4365400000000008</v>
+      </c>
+      <c r="F32">
+        <v>10.3</v>
+      </c>
+      <c r="G32">
+        <v>0.42249999999999999</v>
+      </c>
+      <c r="H32">
+        <v>6.4</v>
+      </c>
+      <c r="I32">
+        <v>0.25600000000000001</v>
+      </c>
+      <c r="J32">
+        <v>1.83</v>
+      </c>
+      <c r="K32">
+        <v>7.0239999999999997E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2">
+        <f>SUM(D24:D32)</f>
+        <v>9663.8999999999978</v>
+      </c>
+      <c r="E33" s="2">
+        <f>SUM(E24:E32)</f>
+        <v>46.85371</v>
+      </c>
+      <c r="F33" s="2">
+        <f t="shared" ref="F33:G33" si="0">SUM(F24:F32)</f>
+        <v>591.31999999999994</v>
+      </c>
+      <c r="G33" s="2">
+        <f t="shared" si="0"/>
+        <v>2.9364999999999997</v>
+      </c>
+      <c r="H33" s="2">
+        <f t="shared" ref="H33" si="1">SUM(H24:H32)</f>
+        <v>374.91999999999996</v>
+      </c>
+      <c r="I33" s="2">
+        <f t="shared" ref="I33" si="2">SUM(I24:I32)</f>
+        <v>1.7725199999999999</v>
+      </c>
+      <c r="J33" s="2">
+        <f t="shared" ref="J33" si="3">SUM(J24:J32)</f>
+        <v>106.95000000000003</v>
+      </c>
+      <c r="K33" s="2">
+        <f t="shared" ref="K33" si="4">SUM(K24:K32)</f>
+        <v>0.61708999999999992</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2">
+        <f>D33/D33</f>
+        <v>1</v>
+      </c>
+      <c r="E34" s="2">
+        <f>D33/E33</f>
+        <v>206.25687912440654</v>
+      </c>
+      <c r="F34" s="2">
+        <f>F33/F33</f>
+        <v>1</v>
+      </c>
+      <c r="G34" s="2">
+        <f>F33/G33</f>
+        <v>201.36897667290992</v>
+      </c>
+      <c r="H34" s="2">
+        <f>H33/H33</f>
+        <v>1</v>
+      </c>
+      <c r="I34" s="2">
+        <f>H33/I33</f>
+        <v>211.51806467628009</v>
+      </c>
+      <c r="J34" s="2">
+        <f>J33/J33</f>
+        <v>1</v>
+      </c>
+      <c r="K34" s="2">
+        <f>J33/K33</f>
+        <v>173.31345508758861</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="7">
+    <mergeCell ref="J22:K22"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="E5:E7"/>
     <mergeCell ref="G5:G9"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="H22:I22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Adding final results and a warning for large images
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="20">
   <si>
     <t>apply_gaussian_kernel</t>
   </si>
@@ -60,9 +60,6 @@
   </si>
   <si>
     <t>Total</t>
-  </si>
-  <si>
-    <t>daimler_800_410</t>
   </si>
   <si>
     <t>GPU (stream for mag/dir)</t>
@@ -186,12 +183,12 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="3"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="3" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -480,7 +477,7 @@
   <dimension ref="A1:K34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -497,35 +494,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="3"/>
-      <c r="B1" s="4" t="s">
+      <c r="A1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+    </row>
+    <row r="2" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-    </row>
-    <row r="2" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="3" t="s">
+      <c r="G2" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -533,16 +530,16 @@
         <v>0</v>
       </c>
       <c r="B3">
-        <v>18.03</v>
+        <v>99.57</v>
       </c>
       <c r="C3">
-        <v>0.20275000000000001</v>
+        <v>0.82864000000000004</v>
       </c>
       <c r="D3">
-        <v>0.19827</v>
+        <v>0.82720000000000005</v>
       </c>
       <c r="F3">
-        <v>0.19964999999999999</v>
+        <v>0.82928000000000002</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -550,16 +547,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>0.71</v>
+        <v>3.99</v>
       </c>
       <c r="C4">
-        <v>0.19885</v>
+        <v>0.82786999999999999</v>
       </c>
       <c r="D4">
-        <v>0.19250999999999999</v>
+        <v>0.82572999999999996</v>
       </c>
       <c r="F4">
-        <v>0.19980999999999999</v>
+        <v>0.83062000000000002</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -567,24 +564,20 @@
         <v>1</v>
       </c>
       <c r="B5">
-        <v>35.85</v>
+        <v>196.63</v>
       </c>
       <c r="C5">
-        <v>0.36656</v>
+        <v>1.19763</v>
       </c>
       <c r="D5">
-        <v>1.0200000000000001E-3</v>
-      </c>
-      <c r="E5" s="1">
-        <f>SUM(C5:C7) - SUM(D5:D7)</f>
-        <v>0.68220999999999998</v>
+        <v>2.3818600000000001</v>
+      </c>
+      <c r="E5" s="4">
+        <f>SUM(C5:C6) - SUM(D5:D6)</f>
+        <v>0.81294999999999984</v>
       </c>
       <c r="F5">
-        <v>8.3000000000000001E-4</v>
-      </c>
-      <c r="G5" s="1">
-        <f>SUM(D5:D9) - SUM(F5:F9)</f>
-        <v>0.24640000000000001</v>
+        <v>2.3845399999999999</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -592,90 +585,85 @@
         <v>2</v>
       </c>
       <c r="B6">
-        <v>34.93</v>
+        <v>191.88</v>
       </c>
       <c r="C6">
-        <v>0.36764999999999998</v>
+        <v>1.99718</v>
       </c>
       <c r="D6">
         <v>0</v>
       </c>
-      <c r="E6" s="1"/>
+      <c r="E6" s="4"/>
       <c r="F6">
         <v>0</v>
       </c>
-      <c r="G6" s="1"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3</v>
       </c>
       <c r="B7">
-        <v>2.83</v>
+        <v>15.83</v>
       </c>
       <c r="C7">
-        <v>5.2639999999999999E-2</v>
+        <v>0.26425999999999999</v>
       </c>
       <c r="D7">
-        <v>0.10362</v>
-      </c>
-      <c r="E7" s="1"/>
+        <v>0.32</v>
+      </c>
       <c r="F7">
-        <v>1.09E-3</v>
-      </c>
-      <c r="G7" s="1"/>
+        <v>1.0198700000000001</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>4</v>
       </c>
       <c r="B8">
-        <v>6.4</v>
+        <v>33.42</v>
       </c>
       <c r="C8">
-        <v>0.16352</v>
+        <v>0.72367999999999999</v>
       </c>
       <c r="D8">
-        <v>0.16186</v>
+        <v>0.72502</v>
       </c>
       <c r="F8">
         <v>0</v>
       </c>
-      <c r="G8" s="1"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>5</v>
       </c>
       <c r="B9">
-        <v>4.22</v>
+        <v>21.54</v>
       </c>
       <c r="C9">
-        <v>6.2560000000000004E-2</v>
+        <v>0.32473999999999997</v>
       </c>
       <c r="D9">
-        <v>6.6619999999999999E-2</v>
+        <v>0.33711999999999998</v>
       </c>
       <c r="F9">
-        <v>8.48E-2</v>
-      </c>
-      <c r="G9" s="1"/>
+        <v>0.33978000000000003</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
       <c r="B10">
-        <v>1.76</v>
+        <v>10.11</v>
       </c>
       <c r="C10">
-        <v>3.6900000000000002E-2</v>
+        <v>0.18626999999999999</v>
       </c>
       <c r="D10">
-        <v>9.2700000000000005E-2</v>
+        <v>0.2399</v>
       </c>
       <c r="F10">
-        <v>9.2060000000000003E-2</v>
+        <v>0.24207999999999999</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -683,109 +671,109 @@
         <v>8</v>
       </c>
       <c r="B11">
-        <v>1.81</v>
+        <v>10.61</v>
       </c>
       <c r="C11">
-        <v>6.7970000000000003E-2</v>
+        <v>0.45373000000000002</v>
       </c>
       <c r="D11">
-        <v>0.16342000000000001</v>
+        <v>0.50953999999999999</v>
       </c>
       <c r="F11">
-        <v>0.11866</v>
+        <v>0.51139000000000001</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" s="1">
         <f>SUM(B3:B11)</f>
-        <v>106.54000000000002</v>
-      </c>
-      <c r="C12" s="2">
+        <v>583.57999999999993</v>
+      </c>
+      <c r="C12" s="1">
         <f>SUM(C3:C11)</f>
-        <v>1.5194000000000001</v>
-      </c>
-      <c r="D12" s="2">
+        <v>6.8040000000000012</v>
+      </c>
+      <c r="D12" s="1">
         <f>SUM(D3:D11)</f>
-        <v>0.98002000000000011</v>
-      </c>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2">
+        <v>6.1663699999999997</v>
+      </c>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1">
         <f>SUM(F3:F11)</f>
-        <v>0.69689999999999996</v>
+        <v>6.1575600000000001</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="2">
+      <c r="A13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="1">
         <f>B12/B12</f>
         <v>1</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="1">
         <f>B12/C12</f>
-        <v>70.119784125312634</v>
-      </c>
-      <c r="D13" s="2">
+        <v>85.770135214579639</v>
+      </c>
+      <c r="D13" s="1">
         <f>B12/D12</f>
-        <v>108.71206710067142</v>
-      </c>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2">
+        <v>94.639147504934016</v>
+      </c>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1">
         <f>B12/F12</f>
-        <v>152.87702683311812</v>
+        <v>94.774553556928382</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="3"/>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="4" t="s">
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4" t="s">
+      <c r="G22" s="3"/>
+      <c r="H22" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G22" s="4"/>
-      <c r="H22" s="4" t="s">
+      <c r="I22" s="3"/>
+      <c r="J22" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="I22" s="4"/>
-      <c r="J22" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="K22" s="4"/>
+      <c r="K22" s="3"/>
     </row>
     <row r="23" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="3"/>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3" t="s">
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E23" s="3" t="s">
+      <c r="E23" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F23" s="3" t="s">
+      <c r="F23" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G23" s="3" t="s">
+      <c r="G23" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H23" s="3" t="s">
+      <c r="H23" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="I23" s="3" t="s">
+      <c r="I23" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="J23" s="3" t="s">
+      <c r="J23" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K23" s="3" t="s">
+      <c r="K23" s="2" t="s">
         <v>10</v>
       </c>
     </row>
@@ -794,28 +782,28 @@
         <v>0</v>
       </c>
       <c r="D24">
-        <v>1629.69</v>
+        <v>1606.42</v>
       </c>
       <c r="E24">
-        <v>17.352029999999999</v>
+        <v>13.21834</v>
       </c>
       <c r="F24">
-        <v>103.37</v>
+        <v>100.47</v>
       </c>
       <c r="G24">
-        <v>1.07213</v>
+        <v>0.82867000000000002</v>
       </c>
       <c r="H24">
-        <v>62.06</v>
+        <v>61.42</v>
       </c>
       <c r="I24">
-        <v>0.64866999999999997</v>
+        <v>0.49852999999999997</v>
       </c>
       <c r="J24">
-        <v>18.739999999999998</v>
+        <v>24.87</v>
       </c>
       <c r="K24">
-        <v>0.20058000000000001</v>
+        <v>0.15445999999999999</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
@@ -823,28 +811,28 @@
         <v>6</v>
       </c>
       <c r="D25">
-        <v>63.61</v>
+        <v>63.66</v>
       </c>
       <c r="E25">
-        <v>12.748799999999999</v>
+        <v>12.529629999999999</v>
       </c>
       <c r="F25">
         <v>3.98</v>
       </c>
       <c r="G25">
-        <v>0.87002000000000002</v>
+        <v>1.1670400000000001</v>
       </c>
       <c r="H25">
         <v>2.39</v>
       </c>
       <c r="I25">
-        <v>0.51500999999999997</v>
+        <v>0.53098000000000001</v>
       </c>
       <c r="J25">
-        <v>0.72</v>
+        <v>0.71</v>
       </c>
       <c r="K25">
-        <v>0.21187</v>
+        <v>0.20221</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
@@ -852,28 +840,28 @@
         <v>1</v>
       </c>
       <c r="D26">
-        <v>3192.68</v>
+        <v>3274.88</v>
       </c>
       <c r="E26">
-        <v>1.6299999999999999E-3</v>
+        <v>38.89658</v>
       </c>
       <c r="F26">
-        <v>197.6</v>
+        <v>195.47</v>
       </c>
       <c r="G26">
-        <v>1.6999999999999999E-3</v>
+        <v>2.3927700000000001</v>
       </c>
       <c r="H26">
-        <v>122.05</v>
+        <v>129.33000000000001</v>
       </c>
       <c r="I26">
-        <v>1.6999999999999999E-3</v>
+        <v>1.4402600000000001</v>
       </c>
       <c r="J26">
-        <v>35.380000000000003</v>
+        <v>35.659999999999997</v>
       </c>
       <c r="K26">
-        <v>8.0000000000000004E-4</v>
+        <v>0.45957999999999999</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
@@ -881,25 +869,25 @@
         <v>2</v>
       </c>
       <c r="D27">
-        <v>3135.95</v>
+        <v>3165.22</v>
       </c>
       <c r="E27">
-        <v>6.7580000000000001E-2</v>
+        <v>22.070080000000001</v>
       </c>
       <c r="F27">
-        <v>194.29</v>
+        <v>190.8</v>
       </c>
       <c r="G27">
-        <v>4.3040000000000002E-2</v>
+        <v>1.0158700000000001</v>
       </c>
       <c r="H27">
-        <v>127.96</v>
+        <v>116.77</v>
       </c>
       <c r="I27">
         <v>0</v>
       </c>
       <c r="J27">
-        <v>34.74</v>
+        <v>34.82</v>
       </c>
       <c r="K27">
         <v>0</v>
@@ -910,28 +898,28 @@
         <v>3</v>
       </c>
       <c r="D28">
-        <v>254.7</v>
+        <v>263.88</v>
       </c>
       <c r="E28">
         <v>0</v>
       </c>
       <c r="F28">
-        <v>16.149999999999999</v>
+        <v>15.77</v>
       </c>
       <c r="G28">
         <v>0</v>
       </c>
       <c r="H28">
-        <v>11.81</v>
+        <v>9.61</v>
       </c>
       <c r="I28">
-        <v>3.0589999999999999E-2</v>
+        <v>0.81206</v>
       </c>
       <c r="J28">
-        <v>3.01</v>
+        <v>3.12</v>
       </c>
       <c r="K28">
-        <v>3.542E-2</v>
+        <v>0.24301</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
@@ -939,25 +927,25 @@
         <v>4</v>
       </c>
       <c r="D29">
-        <v>561.04</v>
+        <v>569.57000000000005</v>
       </c>
       <c r="E29">
-        <v>5.3512599999999999</v>
+        <v>5.39757</v>
       </c>
       <c r="F29">
-        <v>33.979999999999997</v>
+        <v>34.94</v>
       </c>
       <c r="G29">
-        <v>0.33821000000000001</v>
+        <v>0.35926000000000002</v>
       </c>
       <c r="H29">
-        <v>20.36</v>
+        <v>20.73</v>
       </c>
       <c r="I29">
         <v>0</v>
       </c>
       <c r="J29">
-        <v>6.32</v>
+        <v>6.31</v>
       </c>
       <c r="K29">
         <v>0</v>
@@ -968,28 +956,28 @@
         <v>5</v>
       </c>
       <c r="D30">
-        <v>420.45</v>
+        <v>424.7</v>
       </c>
       <c r="E30">
         <v>0</v>
       </c>
       <c r="F30">
-        <v>21.3</v>
+        <v>21.13</v>
       </c>
       <c r="G30">
         <v>0</v>
       </c>
       <c r="H30">
-        <v>15.89</v>
+        <v>15.98</v>
       </c>
       <c r="I30">
-        <v>0.2089</v>
+        <v>0.22489999999999999</v>
       </c>
       <c r="J30">
-        <v>4.29</v>
+        <v>4.7699999999999996</v>
       </c>
       <c r="K30">
-        <v>6.2530000000000002E-2</v>
+        <v>7.7410000000000007E-2</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
@@ -997,28 +985,28 @@
         <v>7</v>
       </c>
       <c r="D31">
-        <v>195.8</v>
+        <v>199.27</v>
       </c>
       <c r="E31">
-        <v>2.8958699999999999</v>
+        <v>3.0142099999999998</v>
       </c>
       <c r="F31">
-        <v>10.35</v>
+        <v>10.28</v>
       </c>
       <c r="G31">
-        <v>0.18890000000000001</v>
+        <v>0.24413000000000001</v>
       </c>
       <c r="H31">
-        <v>6</v>
+        <v>6.04</v>
       </c>
       <c r="I31">
-        <v>0.11165</v>
+        <v>0.17097999999999999</v>
       </c>
       <c r="J31">
-        <v>1.92</v>
+        <v>1.86</v>
       </c>
       <c r="K31">
-        <v>3.5650000000000001E-2</v>
+        <v>9.3119999999999994E-2</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
@@ -1026,117 +1014,116 @@
         <v>8</v>
       </c>
       <c r="D32">
-        <v>209.98</v>
+        <v>222.89</v>
       </c>
       <c r="E32">
-        <v>8.4365400000000008</v>
+        <v>9.6307200000000002</v>
       </c>
       <c r="F32">
-        <v>10.3</v>
+        <v>10.48</v>
       </c>
       <c r="G32">
-        <v>0.42249999999999999</v>
+        <v>0.51097999999999999</v>
       </c>
       <c r="H32">
-        <v>6.4</v>
+        <v>6.26</v>
       </c>
       <c r="I32">
-        <v>0.25600000000000001</v>
+        <v>0.33994000000000002</v>
       </c>
       <c r="J32">
-        <v>1.83</v>
+        <v>1.72</v>
       </c>
       <c r="K32">
-        <v>7.0239999999999997E-2</v>
+        <v>0.13114000000000001</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
+      <c r="A33" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2">
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1">
         <f>SUM(D24:D32)</f>
-        <v>9663.8999999999978</v>
-      </c>
-      <c r="E33" s="2">
+        <v>9790.49</v>
+      </c>
+      <c r="E33" s="1">
         <f>SUM(E24:E32)</f>
-        <v>46.85371</v>
-      </c>
-      <c r="F33" s="2">
+        <v>104.75713</v>
+      </c>
+      <c r="F33" s="1">
         <f t="shared" ref="F33:G33" si="0">SUM(F24:F32)</f>
-        <v>591.31999999999994</v>
-      </c>
-      <c r="G33" s="2">
+        <v>583.32000000000005</v>
+      </c>
+      <c r="G33" s="1">
         <f t="shared" si="0"/>
-        <v>2.9364999999999997</v>
-      </c>
-      <c r="H33" s="2">
+        <v>6.518720000000001</v>
+      </c>
+      <c r="H33" s="1">
         <f t="shared" ref="H33" si="1">SUM(H24:H32)</f>
-        <v>374.91999999999996</v>
-      </c>
-      <c r="I33" s="2">
+        <v>368.53000000000009</v>
+      </c>
+      <c r="I33" s="1">
         <f t="shared" ref="I33" si="2">SUM(I24:I32)</f>
-        <v>1.7725199999999999</v>
-      </c>
-      <c r="J33" s="2">
+        <v>4.0176500000000006</v>
+      </c>
+      <c r="J33" s="1">
         <f t="shared" ref="J33" si="3">SUM(J24:J32)</f>
-        <v>106.95000000000003</v>
-      </c>
-      <c r="K33" s="2">
+        <v>113.84</v>
+      </c>
+      <c r="K33" s="1">
         <f t="shared" ref="K33" si="4">SUM(K24:K32)</f>
-        <v>0.61708999999999992</v>
+        <v>1.36093</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2">
+      <c r="A34" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1">
         <f>D33/D33</f>
         <v>1</v>
       </c>
-      <c r="E34" s="2">
+      <c r="E34" s="1">
         <f>D33/E33</f>
-        <v>206.25687912440654</v>
-      </c>
-      <c r="F34" s="2">
+        <v>93.458936876182079</v>
+      </c>
+      <c r="F34" s="1">
         <f>F33/F33</f>
         <v>1</v>
       </c>
-      <c r="G34" s="2">
+      <c r="G34" s="1">
         <f>F33/G33</f>
-        <v>201.36897667290992</v>
-      </c>
-      <c r="H34" s="2">
+        <v>89.483825045407684</v>
+      </c>
+      <c r="H34" s="1">
         <f>H33/H33</f>
         <v>1</v>
       </c>
-      <c r="I34" s="2">
+      <c r="I34" s="1">
         <f>H33/I33</f>
-        <v>211.51806467628009</v>
-      </c>
-      <c r="J34" s="2">
+        <v>91.727751297400232</v>
+      </c>
+      <c r="J34" s="1">
         <f>J33/J33</f>
         <v>1</v>
       </c>
-      <c r="K34" s="2">
+      <c r="K34" s="1">
         <f>J33/K33</f>
-        <v>173.31345508758861</v>
+        <v>83.648681416384392</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="6">
     <mergeCell ref="J22:K22"/>
     <mergeCell ref="B1:C1"/>
-    <mergeCell ref="E5:E7"/>
-    <mergeCell ref="G5:G9"/>
     <mergeCell ref="D22:E22"/>
     <mergeCell ref="F22:G22"/>
     <mergeCell ref="H22:I22"/>
+    <mergeCell ref="E5:E6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>